<commit_message>
[Adobe] Mapping Version Fix
</commit_message>
<xml_diff>
--- a/tools/excel/adobe/mappings/mapping-adobe-ccf-v5-to-bsi-c5-2020.xlsx
+++ b/tools/excel/adobe/mappings/mapping-adobe-ccf-v5-to-bsi-c5-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\adobe\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839AB523-950A-4B34-A712-F81DAE5B6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB338584-3B03-43E7-8549-45341C0BDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5130" yWindow="-12960" windowWidth="20865" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7738,7 +7738,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7767,7 +7767,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>